<commit_message>
Added figures and maps
</commit_message>
<xml_diff>
--- a/SPF_surveys_110321.xlsx
+++ b/SPF_surveys_110321.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="558">
   <si>
     <t>Survey</t>
   </si>
@@ -1808,9 +1808,6 @@
     <t>Sardinella brasiliensis</t>
   </si>
   <si>
-    <t>California Current</t>
-  </si>
-  <si>
     <t>Newfoundland-Labrador Shelf</t>
   </si>
   <si>
@@ -1919,8 +1916,13 @@
     <t>Kattegat</t>
   </si>
   <si>
-    <t xml:space="preserve">North Sea
-</t>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Baltic Sea</t>
   </si>
 </sst>
 </file>
@@ -5036,10 +5038,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5053,74 +5055,92 @@
     <col min="7" max="7" width="27.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>549</v>
+      <c r="H1" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>556</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>440</v>
+        <v>557</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>277</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>406</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>468</v>
       </c>
+      <c r="H2">
+        <v>19.863299999999999</v>
+      </c>
+      <c r="I2">
+        <v>58.488</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>440</v>
+        <v>557</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>266</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
+      </c>
+      <c r="H3">
+        <v>19.863299999999999</v>
+      </c>
+      <c r="I3">
+        <v>58.488</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
@@ -5128,20 +5148,26 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>476</v>
       </c>
+      <c r="H4">
+        <v>37.106400000000001</v>
+      </c>
+      <c r="I4">
+        <v>74.988399999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>71</v>
       </c>
@@ -5149,20 +5175,26 @@
         <v>394</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>468</v>
       </c>
+      <c r="H5">
+        <v>37.106400000000001</v>
+      </c>
+      <c r="I5">
+        <v>74.988399999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
@@ -5170,22 +5202,28 @@
         <v>398</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>420</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H6">
+        <v>-3.1631999999999998</v>
+      </c>
+      <c r="I6">
+        <v>45.557000000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>454</v>
       </c>
@@ -5193,114 +5231,144 @@
         <v>460</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G7" s="4"/>
+      <c r="H7">
+        <v>-126</v>
+      </c>
+      <c r="I7">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>519</v>
+        <v>454</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>396</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>479</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
+      </c>
+      <c r="H8">
+        <v>-126</v>
+      </c>
+      <c r="I8">
+        <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>454</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>418</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H9">
+        <v>-126</v>
+      </c>
+      <c r="I9">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>404</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>487</v>
       </c>
+      <c r="H10">
+        <v>-126</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>414</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H11">
+        <v>-126</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>414</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>478</v>
@@ -5308,52 +5376,70 @@
       <c r="G12" s="4" t="s">
         <v>473</v>
       </c>
+      <c r="H12">
+        <v>-126</v>
+      </c>
+      <c r="I12">
+        <v>40</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>414</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>478</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
+      </c>
+      <c r="H13">
+        <v>-126</v>
+      </c>
+      <c r="I13">
+        <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>414</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>412</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H14">
+        <v>-126</v>
+      </c>
+      <c r="I14">
+        <v>40</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>443</v>
       </c>
@@ -5361,37 +5447,49 @@
         <v>398</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>467</v>
       </c>
+      <c r="H15">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I15">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>443</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H16">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I16">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>443</v>
       </c>
@@ -5399,539 +5497,695 @@
         <v>398</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="7"/>
       <c r="F17" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>467</v>
       </c>
+      <c r="H17">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I17">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>443</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>286</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H18">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I18">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>443</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>277</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>407</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H19">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I19">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>433</v>
+    <row r="20" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>443</v>
       </c>
       <c r="B20" s="33" t="s">
         <v>397</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D20" s="33" t="s">
         <v>410</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>468</v>
       </c>
+      <c r="H20">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I20">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>433</v>
+    <row r="21" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>443</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>401</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H21">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I21">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>433</v>
+    <row r="22" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>443</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>401</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>468</v>
       </c>
+      <c r="H22">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I22">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>433</v>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>443</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>468</v>
       </c>
+      <c r="H23">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I23">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="24" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>433</v>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>443</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H24">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I24">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="25" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>433</v>
+    <row r="25" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>443</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>398</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>420</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H25">
+        <v>-8.2502999999999993</v>
+      </c>
+      <c r="I25">
+        <v>49.070500000000003</v>
+      </c>
     </row>
-    <row r="26" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H26">
+        <v>0.35709999999999997</v>
+      </c>
+      <c r="I26">
+        <v>50.134700000000002</v>
+      </c>
     </row>
-    <row r="27" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>408</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>476</v>
       </c>
+      <c r="H27">
+        <v>0.35709999999999997</v>
+      </c>
+      <c r="I27">
+        <v>50.134700000000002</v>
+      </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G28" s="4"/>
+      <c r="H28">
+        <v>-176.1395</v>
+      </c>
+      <c r="I28">
+        <v>56.907299999999999</v>
+      </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G29" s="4"/>
+      <c r="H29">
+        <v>-176.1395</v>
+      </c>
+      <c r="I29">
+        <v>56.907299999999999</v>
+      </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H30">
+        <v>-176.1395</v>
+      </c>
+      <c r="I30">
+        <v>56.907299999999999</v>
+      </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>327</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G31" s="4"/>
+      <c r="H31">
+        <v>-144</v>
+      </c>
+      <c r="I31">
+        <v>57</v>
+      </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>327</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G32" s="4"/>
+      <c r="H32">
+        <v>-144</v>
+      </c>
+      <c r="I32">
+        <v>57</v>
+      </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>327</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G33" s="4"/>
+      <c r="H33">
+        <v>-144</v>
+      </c>
+      <c r="I33">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>327</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H34">
+        <v>-144</v>
+      </c>
+      <c r="I34">
+        <v>57</v>
+      </c>
     </row>
-    <row r="35" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>491</v>
+        <v>327</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>414</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>412</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H35">
+        <v>-144</v>
+      </c>
+      <c r="I35">
+        <v>57</v>
+      </c>
     </row>
-    <row r="36" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>491</v>
+        <v>327</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>400</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>294</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H36">
+        <v>-144</v>
+      </c>
+      <c r="I36">
+        <v>57</v>
+      </c>
     </row>
-    <row r="37" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B37" s="25" t="s">
         <v>398</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>420</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H37">
+        <v>-12.0876</v>
+      </c>
+      <c r="I37">
+        <v>40.482999999999997</v>
+      </c>
     </row>
-    <row r="38" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>42</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H38">
+        <v>11.3004</v>
+      </c>
+      <c r="I38">
+        <v>56.951999999999998</v>
+      </c>
     </row>
-    <row r="39" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>408</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>476</v>
       </c>
+      <c r="H39">
+        <v>11.3004</v>
+      </c>
+      <c r="I39">
+        <v>56.951999999999998</v>
+      </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H40">
+        <v>-50</v>
+      </c>
+      <c r="I40">
+        <v>51</v>
+      </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B41" s="32" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="19" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G41" s="19" t="s">
         <v>466</v>
       </c>
+      <c r="H41">
+        <v>-50</v>
+      </c>
+      <c r="I41">
+        <v>51</v>
+      </c>
     </row>
-    <row r="42" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>438</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>277</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>468</v>
       </c>
+      <c r="H42">
+        <v>3.5156000000000001</v>
+      </c>
+      <c r="I42">
+        <v>56.511000000000003</v>
+      </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>438</v>
       </c>
@@ -5939,20 +6193,26 @@
         <v>3</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H43">
+        <v>3.5156000000000001</v>
+      </c>
+      <c r="I43">
+        <v>56.511000000000003</v>
+      </c>
     </row>
-    <row r="44" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>438</v>
       </c>
@@ -5960,22 +6220,28 @@
         <v>3</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>42</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H44">
+        <v>3.5156000000000001</v>
+      </c>
+      <c r="I44">
+        <v>56.511000000000003</v>
+      </c>
     </row>
-    <row r="45" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>438</v>
       </c>
@@ -5983,66 +6249,84 @@
         <v>3</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>408</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>476</v>
       </c>
+      <c r="H45">
+        <v>3.5156000000000001</v>
+      </c>
+      <c r="I45">
+        <v>56.511000000000003</v>
+      </c>
     </row>
-    <row r="46" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>556</v>
+        <v>438</v>
       </c>
       <c r="B46" s="25" t="s">
         <v>277</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>407</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H46">
+        <v>3.5156000000000001</v>
+      </c>
+      <c r="I46">
+        <v>56.511000000000003</v>
+      </c>
     </row>
-    <row r="47" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B47" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D47" s="31"/>
       <c r="E47" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
+      </c>
+      <c r="H47">
+        <v>3.5156000000000001</v>
+      </c>
+      <c r="I47">
+        <v>56.511000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>325</v>
       </c>
@@ -6050,18 +6334,24 @@
         <v>395</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D48" s="31"/>
       <c r="E48" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>266</v>
       </c>
       <c r="G48" s="6"/>
+      <c r="H48">
+        <v>-70</v>
+      </c>
+      <c r="I48">
+        <v>40</v>
+      </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>325</v>
       </c>
@@ -6069,18 +6359,26 @@
         <v>3</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="G49" s="4"/>
+        <v>531</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H49">
+        <v>-70</v>
+      </c>
+      <c r="I49">
+        <v>40</v>
+      </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>495</v>
       </c>
@@ -6088,167 +6386,215 @@
         <v>3</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H50">
+        <v>12</v>
+      </c>
+      <c r="I50">
+        <v>69</v>
+      </c>
     </row>
-    <row r="51" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>457</v>
+        <v>495</v>
       </c>
       <c r="B51" s="25" t="s">
         <v>277</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G51" s="4"/>
+      <c r="H51">
+        <v>12</v>
+      </c>
+      <c r="I51">
+        <v>69</v>
+      </c>
     </row>
-    <row r="52" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>457</v>
+        <v>495</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H52">
+        <v>12</v>
+      </c>
+      <c r="I52">
+        <v>69</v>
+      </c>
     </row>
-    <row r="53" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>457</v>
+        <v>495</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="H53">
+        <v>12</v>
+      </c>
+      <c r="I53">
+        <v>69</v>
+      </c>
     </row>
-    <row r="54" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>457</v>
+        <v>495</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>476</v>
       </c>
+      <c r="H54">
+        <v>12</v>
+      </c>
+      <c r="I54">
+        <v>69</v>
+      </c>
     </row>
-    <row r="55" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B55" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>42</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>467</v>
       </c>
+      <c r="H55">
+        <v>9.9314999999999998</v>
+      </c>
+      <c r="I55">
+        <v>58.3523</v>
+      </c>
     </row>
-    <row r="56" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B56" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>408</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>476</v>
       </c>
+      <c r="H56">
+        <v>9.9314999999999998</v>
+      </c>
+      <c r="I56">
+        <v>58.3523</v>
+      </c>
     </row>
-    <row r="57" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>395</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D57" s="31"/>
       <c r="E57" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>266</v>
       </c>
       <c r="G57" s="6"/>
+      <c r="H57">
+        <v>-76</v>
+      </c>
+      <c r="I57">
+        <v>30</v>
+      </c>
     </row>
-    <row r="58" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="38" t="s">
         <v>510</v>
       </c>
@@ -6256,63 +6602,81 @@
         <v>512</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D58" s="39"/>
       <c r="E58" s="38" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F58" s="38" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G58" s="38" t="s">
         <v>487</v>
       </c>
+      <c r="H58">
+        <v>155</v>
+      </c>
+      <c r="I58">
+        <v>-35</v>
+      </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B59" s="25" t="s">
         <v>295</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>371</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G59" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="H59">
+        <v>-45</v>
+      </c>
+      <c r="I59">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>530</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>531</v>
       </c>
       <c r="B60" s="25" t="s">
         <v>295</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>371</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
+      </c>
+      <c r="H60">
+        <v>-45</v>
+      </c>
+      <c r="I60">
+        <v>-30</v>
       </c>
     </row>
   </sheetData>
@@ -25010,12 +25374,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25191,21 +25558,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59FF985-1183-4834-8086-C77161FBE6F8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{006CA9B9-CD5F-42FA-AEB9-AB45473197E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25229,17 +25601,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{006CA9B9-CD5F-42FA-AEB9-AB45473197E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59FF985-1183-4834-8086-C77161FBE6F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>